<commit_message>
Foi feito o sistema de apagar lista junto ao excel agora para todas as listas, foi feito uma função de popup para erros comuns onde vai ser reutilizada quando necessário
</commit_message>
<xml_diff>
--- a/storage/listaPERFUMARIA.xlsx
+++ b/storage/listaPERFUMARIA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,43 +470,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>07/07/2023</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>100.00</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>